<commit_message>
Updated code to make new graphml files
</commit_message>
<xml_diff>
--- a/grp_edgelists/grp-edgelist.xlsx
+++ b/grp_edgelists/grp-edgelist.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annie Armstrong\Documents\Github\mindmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annie Armstrong\Documents\Github\mindmap\grp_edgelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3D1E38B-C33B-4D64-97C7-AFDDF1A0E0F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2992844B-B7C2-43E8-B5FA-7953D3E654D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{AFA33BF0-5886-4B64-BE64-14EDB69C8799}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{AFA33BF0-5886-4B64-BE64-14EDB69C8799}"/>
   </bookViews>
   <sheets>
-    <sheet name="MWSeptGroup" sheetId="1" r:id="rId1"/>
+    <sheet name="Group list" sheetId="1" r:id="rId1"/>
+    <sheet name="Individual lists" sheetId="2" r:id="rId2"/>
+    <sheet name="StudentIDLookup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="184">
   <si>
     <t>Edge</t>
   </si>
@@ -331,6 +333,261 @@
   </si>
   <si>
     <t>TTh</t>
+  </si>
+  <si>
+    <t>StudentID</t>
+  </si>
+  <si>
+    <t>Ricky</t>
+  </si>
+  <si>
+    <t>1MW</t>
+  </si>
+  <si>
+    <t>2MW</t>
+  </si>
+  <si>
+    <t>Bronx River</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>LaGuardia</t>
+  </si>
+  <si>
+    <t>6 Train</t>
+  </si>
+  <si>
+    <t>Pelham Bay Park</t>
+  </si>
+  <si>
+    <t>Time Square</t>
+  </si>
+  <si>
+    <t>Mall</t>
+  </si>
+  <si>
+    <t>Bronx River Alliance</t>
+  </si>
+  <si>
+    <t>Hyde</t>
+  </si>
+  <si>
+    <t>Bronx River Parkway</t>
+  </si>
+  <si>
+    <t>Jacobi Hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bronx River </t>
+  </si>
+  <si>
+    <t>Brother Islands</t>
+  </si>
+  <si>
+    <t>Meliza</t>
+  </si>
+  <si>
+    <t>3MW</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Returner</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>StudentStatus</t>
+  </si>
+  <si>
+    <t>Fishing</t>
+  </si>
+  <si>
+    <t>Falling</t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Fun</t>
+  </si>
+  <si>
+    <t>Birding</t>
+  </si>
+  <si>
+    <t>Site seeing</t>
+  </si>
+  <si>
+    <t>Kayaking</t>
+  </si>
+  <si>
+    <t>Swaying</t>
+  </si>
+  <si>
+    <t>Qualitative Code</t>
+  </si>
+  <si>
+    <t>4MW</t>
+  </si>
+  <si>
+    <t>Creatures</t>
+  </si>
+  <si>
+    <t>Eels</t>
+  </si>
+  <si>
+    <t>Starfish</t>
+  </si>
+  <si>
+    <t>Riverside</t>
+  </si>
+  <si>
+    <t>Mouctar</t>
+  </si>
+  <si>
+    <t>Creatures dying out</t>
+  </si>
+  <si>
+    <t>Views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Views </t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>In my bag</t>
+  </si>
+  <si>
+    <t>Happens all the time</t>
+  </si>
+  <si>
+    <t>Dangerous</t>
+  </si>
+  <si>
+    <t>Dead bodies</t>
+  </si>
+  <si>
+    <t>Leaving Bronx</t>
+  </si>
+  <si>
+    <t>College?</t>
+  </si>
+  <si>
+    <t>Peace Corps</t>
+  </si>
+  <si>
+    <t>5MW</t>
+  </si>
+  <si>
+    <t>Veronica</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Avoiding</t>
+  </si>
+  <si>
+    <t>My mom</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>New friends</t>
+  </si>
+  <si>
+    <t>Photos</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>I'm always hungry</t>
+  </si>
+  <si>
+    <t>Saving</t>
+  </si>
+  <si>
+    <t>Afterschool</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Depression &amp; Stress</t>
+  </si>
+  <si>
+    <t>Solutions</t>
+  </si>
+  <si>
+    <t>Concluding</t>
+  </si>
+  <si>
+    <t>Environmental</t>
+  </si>
+  <si>
+    <t>Hands hurt</t>
+  </si>
+  <si>
+    <t>Getting wet</t>
+  </si>
+  <si>
+    <t>Smells</t>
+  </si>
+  <si>
+    <t>Crotona</t>
+  </si>
+  <si>
+    <t>Antics</t>
+  </si>
+  <si>
+    <t>Bronx</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>Ew</t>
+  </si>
+  <si>
+    <t>Starlight Park</t>
+  </si>
+  <si>
+    <t>Bronx Zoo</t>
+  </si>
+  <si>
+    <t>Sad animals</t>
+  </si>
+  <si>
+    <t>Walking</t>
+  </si>
+  <si>
+    <t>I'm a bird</t>
   </si>
 </sst>
 </file>
@@ -700,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75B9E74-F85C-4AA5-B2A7-0BAD20C99193}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1966,4 +2223,1984 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCFCEF4-088F-4F4C-BAD0-BADB2CC3EDCA}">
+  <dimension ref="A1:Q95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78:F95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" t="s">
+        <v>134</v>
+      </c>
+      <c r="F42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" t="s">
+        <v>134</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" t="s">
+        <v>151</v>
+      </c>
+      <c r="F48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" t="s">
+        <v>151</v>
+      </c>
+      <c r="F49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" t="s">
+        <v>151</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>149</v>
+      </c>
+      <c r="B53" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" t="s">
+        <v>151</v>
+      </c>
+      <c r="F53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" t="s">
+        <v>151</v>
+      </c>
+      <c r="F54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" t="s">
+        <v>151</v>
+      </c>
+      <c r="F55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" t="s">
+        <v>151</v>
+      </c>
+      <c r="F57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" t="s">
+        <v>151</v>
+      </c>
+      <c r="F58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" t="s">
+        <v>151</v>
+      </c>
+      <c r="F59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" t="s">
+        <v>151</v>
+      </c>
+      <c r="F61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" t="s">
+        <v>151</v>
+      </c>
+      <c r="F62" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" t="s">
+        <v>151</v>
+      </c>
+      <c r="F63" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" t="s">
+        <v>151</v>
+      </c>
+      <c r="F64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" t="s">
+        <v>162</v>
+      </c>
+      <c r="C65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" t="s">
+        <v>151</v>
+      </c>
+      <c r="F65" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>162</v>
+      </c>
+      <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" t="s">
+        <v>151</v>
+      </c>
+      <c r="F66" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+      <c r="E67" t="s">
+        <v>151</v>
+      </c>
+      <c r="F67" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" t="s">
+        <v>35</v>
+      </c>
+      <c r="E68" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69" t="s">
+        <v>151</v>
+      </c>
+      <c r="F69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B71" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" t="s">
+        <v>35</v>
+      </c>
+      <c r="E71" t="s">
+        <v>151</v>
+      </c>
+      <c r="F71" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>165</v>
+      </c>
+      <c r="B72" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" t="s">
+        <v>35</v>
+      </c>
+      <c r="E72" t="s">
+        <v>151</v>
+      </c>
+      <c r="F72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>166</v>
+      </c>
+      <c r="B73" t="s">
+        <v>167</v>
+      </c>
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" t="s">
+        <v>151</v>
+      </c>
+      <c r="F73" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>167</v>
+      </c>
+      <c r="B74" t="s">
+        <v>168</v>
+      </c>
+      <c r="C74" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" t="s">
+        <v>35</v>
+      </c>
+      <c r="E74" t="s">
+        <v>151</v>
+      </c>
+      <c r="F74" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" t="s">
+        <v>169</v>
+      </c>
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" t="s">
+        <v>35</v>
+      </c>
+      <c r="E75" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>49</v>
+      </c>
+      <c r="B76" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D76" t="s">
+        <v>35</v>
+      </c>
+      <c r="E76" t="s">
+        <v>151</v>
+      </c>
+      <c r="F76" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>170</v>
+      </c>
+      <c r="B77" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" t="s">
+        <v>35</v>
+      </c>
+      <c r="E77" t="s">
+        <v>151</v>
+      </c>
+      <c r="F77" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" t="s">
+        <v>151</v>
+      </c>
+      <c r="F78" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" t="s">
+        <v>35</v>
+      </c>
+      <c r="E79" t="s">
+        <v>151</v>
+      </c>
+      <c r="F79" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>172</v>
+      </c>
+      <c r="B80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" t="s">
+        <v>35</v>
+      </c>
+      <c r="E81" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>174</v>
+      </c>
+      <c r="B82" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D82" t="s">
+        <v>35</v>
+      </c>
+      <c r="E82" t="s">
+        <v>151</v>
+      </c>
+      <c r="F82" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" t="s">
+        <v>31</v>
+      </c>
+      <c r="D83" t="s">
+        <v>35</v>
+      </c>
+      <c r="E83" t="s">
+        <v>151</v>
+      </c>
+      <c r="F83" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" t="s">
+        <v>31</v>
+      </c>
+      <c r="D84" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" t="s">
+        <v>151</v>
+      </c>
+      <c r="F84" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" t="s">
+        <v>31</v>
+      </c>
+      <c r="D85" t="s">
+        <v>35</v>
+      </c>
+      <c r="E85" t="s">
+        <v>151</v>
+      </c>
+      <c r="F85" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" t="s">
+        <v>31</v>
+      </c>
+      <c r="D86" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86" t="s">
+        <v>151</v>
+      </c>
+      <c r="F86" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87" t="s">
+        <v>31</v>
+      </c>
+      <c r="D87" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" t="s">
+        <v>151</v>
+      </c>
+      <c r="F87" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" t="s">
+        <v>31</v>
+      </c>
+      <c r="D88" t="s">
+        <v>35</v>
+      </c>
+      <c r="E88" t="s">
+        <v>151</v>
+      </c>
+      <c r="F88" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89" t="s">
+        <v>179</v>
+      </c>
+      <c r="C89" t="s">
+        <v>31</v>
+      </c>
+      <c r="D89" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" t="s">
+        <v>151</v>
+      </c>
+      <c r="F89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>96</v>
+      </c>
+      <c r="B90" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" t="s">
+        <v>31</v>
+      </c>
+      <c r="D90" t="s">
+        <v>35</v>
+      </c>
+      <c r="E90" t="s">
+        <v>151</v>
+      </c>
+      <c r="F90" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E91" t="s">
+        <v>151</v>
+      </c>
+      <c r="F91" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" t="s">
+        <v>31</v>
+      </c>
+      <c r="D92" t="s">
+        <v>35</v>
+      </c>
+      <c r="E92" t="s">
+        <v>151</v>
+      </c>
+      <c r="F92" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" t="s">
+        <v>31</v>
+      </c>
+      <c r="D93" t="s">
+        <v>35</v>
+      </c>
+      <c r="E93" t="s">
+        <v>151</v>
+      </c>
+      <c r="F93" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" t="s">
+        <v>35</v>
+      </c>
+      <c r="E94" t="s">
+        <v>151</v>
+      </c>
+      <c r="F94" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>183</v>
+      </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" t="s">
+        <v>35</v>
+      </c>
+      <c r="E95" t="s">
+        <v>151</v>
+      </c>
+      <c r="F95" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8E9D17-3AF3-4FF9-AA84-6EF977D876DA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>